<commit_message>
update Zeituebersicht Andreas Z
</commit_message>
<xml_diff>
--- a/doc/Zeituebersicht.xlsx
+++ b/doc/Zeituebersicht.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreas/Documents/Privat/Bildung/03_Studium/06_SoSe17/Vorlesungen/DT/00_git/dt_it6_ss2017/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreas/Documents/Privat/Bildung/03_Studium/06_SoSe17/Vorlesungen/DT/00_git/DT_IT6_SS2017/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="31">
   <si>
     <t>Arbeitszeittabelle</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Mindmap: Weitere Routen-Berechnungen</t>
+  </si>
+  <si>
+    <t>Entwicklungsstart: Route-Library</t>
+  </si>
+  <si>
+    <t>Git-Repository Problembehebungen (Pull-Requests, Merges...)</t>
   </si>
 </sst>
 </file>
@@ -249,7 +255,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -291,6 +297,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -791,8 +806,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Uhrzeit37" displayName="Uhrzeit37" ref="B8:H13" totalsRowShown="0" headerRowDxfId="7" headerRowCellStyle="Heading 3">
-  <autoFilter ref="B8:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Uhrzeit37" displayName="Uhrzeit37" ref="B8:H15" totalsRowShown="0" headerRowDxfId="7" headerRowCellStyle="Heading 3">
+  <autoFilter ref="B8:H15"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Datumsangaben" dataDxfId="6"/>
     <tableColumn id="7" name="Thema" dataDxfId="5"/>
@@ -2149,20 +2164,20 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H13"/>
+  <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" customWidth="1"/>
     <col min="4" max="4" width="26.1640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="32" style="9" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="9" customWidth="1"/>
     <col min="7" max="7" width="26.33203125" style="9" customWidth="1"/>
     <col min="8" max="8" width="23.5" style="11" customWidth="1"/>
   </cols>
@@ -2203,7 +2218,7 @@
     <row r="6" spans="2:8" ht="26" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <f>SUBTOTAL(109,Uhrzeit37[Arbeitsstunden])</f>
-        <v>7.4999999999999973</v>
+        <v>9.8333333333333304</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -2342,6 +2357,46 @@
       <c r="H13" s="10">
         <f>IFERROR(IF(COUNT(Uhrzeit37[[#This Row],[Anwesenheitszeit]:[Abwesenheitszeit]])=4,(IF(Uhrzeit37[[#This Row],[Abwesenheitszeit]]&lt;Uhrzeit37[[#This Row],[Anwesenheitszeit]],1,0)+Uhrzeit37[[#This Row],[Abwesenheitszeit]])-Uhrzeit37[[#This Row],[Ende der Mittagspause]]+Uhrzeit37[[#This Row],[Beginn der Mittagspause]]-Uhrzeit37[[#This Row],[Anwesenheitszeit]],IF(AND(LEN(Uhrzeit37[[#This Row],[Anwesenheitszeit]])&lt;&gt;0,LEN(Uhrzeit37[[#This Row],[Abwesenheitszeit]])&lt;&gt;0),(IF(Uhrzeit37[[#This Row],[Abwesenheitszeit]]&lt;Uhrzeit37[[#This Row],[Anwesenheitszeit]],1,0)+Uhrzeit37[[#This Row],[Abwesenheitszeit]])-Uhrzeit37[[#This Row],[Anwesenheitszeit]],0))*24,0)</f>
         <v>3.4999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="15">
+        <v>42829</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="H14" s="11">
+        <f>IFERROR(IF(COUNT(Uhrzeit37[[#This Row],[Anwesenheitszeit]:[Abwesenheitszeit]])=4,(IF(Uhrzeit37[[#This Row],[Abwesenheitszeit]]&lt;Uhrzeit37[[#This Row],[Anwesenheitszeit]],1,0)+Uhrzeit37[[#This Row],[Abwesenheitszeit]])-Uhrzeit37[[#This Row],[Ende der Mittagspause]]+Uhrzeit37[[#This Row],[Beginn der Mittagspause]]-Uhrzeit37[[#This Row],[Anwesenheitszeit]],IF(AND(LEN(Uhrzeit37[[#This Row],[Anwesenheitszeit]])&lt;&gt;0,LEN(Uhrzeit37[[#This Row],[Abwesenheitszeit]])&lt;&gt;0),(IF(Uhrzeit37[[#This Row],[Abwesenheitszeit]]&lt;Uhrzeit37[[#This Row],[Anwesenheitszeit]],1,0)+Uhrzeit37[[#This Row],[Abwesenheitszeit]])-Uhrzeit37[[#This Row],[Anwesenheitszeit]],0))*24,0)</f>
+        <v>1.9999999999999982</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="15">
+        <v>42836</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="17">
+        <v>0.375</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="H15" s="11">
+        <f>IFERROR(IF(COUNT(Uhrzeit37[[#This Row],[Anwesenheitszeit]:[Abwesenheitszeit]])=4,(IF(Uhrzeit37[[#This Row],[Abwesenheitszeit]]&lt;Uhrzeit37[[#This Row],[Anwesenheitszeit]],1,0)+Uhrzeit37[[#This Row],[Abwesenheitszeit]])-Uhrzeit37[[#This Row],[Ende der Mittagspause]]+Uhrzeit37[[#This Row],[Beginn der Mittagspause]]-Uhrzeit37[[#This Row],[Anwesenheitszeit]],IF(AND(LEN(Uhrzeit37[[#This Row],[Anwesenheitszeit]])&lt;&gt;0,LEN(Uhrzeit37[[#This Row],[Abwesenheitszeit]])&lt;&gt;0),(IF(Uhrzeit37[[#This Row],[Abwesenheitszeit]]&lt;Uhrzeit37[[#This Row],[Anwesenheitszeit]],1,0)+Uhrzeit37[[#This Row],[Abwesenheitszeit]])-Uhrzeit37[[#This Row],[Anwesenheitszeit]],0))*24,0)</f>
+        <v>0.33333333333333348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>